<commit_message>
icon and links added
</commit_message>
<xml_diff>
--- a/excel/novenyes/novenyek_megoldas.xlsx
+++ b/excel/novenyes/novenyek_megoldas.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Munkalap" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="pontozas" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Munkalap" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="pontozas" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -102,11 +102,12 @@
     <numFmt numFmtId="166" formatCode="0.00&quot; cm&quot;"/>
     <numFmt numFmtId="167" formatCode="0%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -128,10 +129,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -209,39 +217,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,7 +325,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -357,12 +365,14 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="hu-HU" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr b="0" lang="hu-HU" sz="1000" strike="noStrike" u="none">
+                    <a:uFillTx/>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -403,7 +413,7 @@
             <c:numRef>
               <c:f>Munkalap!$E$2:$E$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2.5</c:v>
@@ -426,17 +436,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="22541237"/>
-        <c:axId val="53033474"/>
+        <c:axId val="28379567"/>
+        <c:axId val="5213956"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="22541237"/>
+        <c:axId val="28379567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -452,13 +462,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="hu-HU" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr b="0" lang="hu-HU" sz="1000" strike="noStrike" u="none">
+                <a:uFillTx/>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53033474"/>
+        <c:crossAx val="5213956"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -466,7 +477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53033474"/>
+        <c:axId val="5213956"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -481,7 +492,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -497,13 +508,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="hu-HU" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr b="0" lang="hu-HU" sz="1000" strike="noStrike" u="none">
+                <a:uFillTx/>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22541237"/>
+        <c:crossAx val="28379567"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -530,7 +542,8 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" lang="hu-HU" sz="1000" spc="-1" strike="noStrike">
+            <a:defRPr b="0" lang="hu-HU" sz="1000" strike="noStrike" u="none">
+              <a:uFillTx/>
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
@@ -551,7 +564,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -563,12 +576,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="hu-HU" sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+                <a:uFillTx/>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="hu-HU" sz="1300" spc="-1" strike="noStrike">
+              <a:rPr b="0" lang="hu-HU" sz="1300" strike="noStrike" u="none">
+                <a:uFillTx/>
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Hónap végén mért magasság</a:t>
@@ -591,10 +606,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.240952559534971"/>
-          <c:y val="0.131777777777778"/>
-          <c:w val="0.488030501906369"/>
-          <c:h val="0.867555555555555"/>
+          <c:x val="0.240963855421687"/>
+          <c:y val="0.131802940417849"/>
+          <c:w val="0.48802438670344"/>
+          <c:h val="0.867423265411401"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -678,17 +693,20 @@
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
               <c:txPr>
                 <a:bodyPr wrap="none"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr b="1" lang="hu-HU" sz="1400" spc="-1" strike="noStrike">
+                    <a:defRPr b="1" lang="hu-HU" sz="1400" strike="noStrike" u="none">
                       <a:solidFill>
                         <a:srgbClr val="ffffff"/>
                       </a:solidFill>
+                      <a:uFillTx/>
                       <a:latin typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
@@ -704,15 +722,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
               <c:txPr>
                 <a:bodyPr wrap="none"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr b="1" lang="hu-HU" sz="1400" spc="-1" strike="noStrike">
+                    <a:defRPr b="1" lang="hu-HU" sz="1400" strike="noStrike" u="none">
                       <a:solidFill>
                         <a:srgbClr val="ffffff"/>
                       </a:solidFill>
+                      <a:uFillTx/>
                       <a:latin typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
@@ -728,15 +748,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
               <c:txPr>
                 <a:bodyPr wrap="none"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr b="1" lang="hu-HU" sz="1400" spc="-1" strike="noStrike">
+                    <a:defRPr b="1" lang="hu-HU" sz="1400" strike="noStrike" u="none">
                       <a:solidFill>
                         <a:srgbClr val="ffffff"/>
                       </a:solidFill>
+                      <a:uFillTx/>
                       <a:latin typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
@@ -752,15 +774,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
               <c:txPr>
                 <a:bodyPr wrap="none"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr b="1" lang="hu-HU" sz="1400" spc="-1" strike="noStrike">
+                    <a:defRPr b="1" lang="hu-HU" sz="1400" strike="noStrike" u="none">
                       <a:solidFill>
                         <a:srgbClr val="ffffff"/>
                       </a:solidFill>
+                      <a:uFillTx/>
                       <a:latin typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
@@ -776,15 +800,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
               <c:txPr>
                 <a:bodyPr wrap="none"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr b="1" lang="hu-HU" sz="1400" spc="-1" strike="noStrike">
+                    <a:defRPr b="1" lang="hu-HU" sz="1400" strike="noStrike" u="none">
                       <a:solidFill>
                         <a:srgbClr val="ffffff"/>
                       </a:solidFill>
+                      <a:uFillTx/>
                       <a:latin typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
@@ -803,10 +829,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" lang="hu-HU" sz="1400" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" lang="hu-HU" sz="1400" strike="noStrike" u="none">
                     <a:solidFill>
                       <a:srgbClr val="ffffff"/>
                     </a:solidFill>
+                    <a:uFillTx/>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
@@ -892,7 +919,8 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" lang="hu-HU" sz="1000" spc="-1" strike="noStrike">
+            <a:defRPr b="0" lang="hu-HU" sz="1000" strike="noStrike" u="none">
+              <a:uFillTx/>
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
@@ -900,6 +928,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -923,9 +952,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1916280</xdr:colOff>
+      <xdr:colOff>1915920</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -933,8 +962,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="237960" y="3231000"/>
-        <a:ext cx="5012640" cy="2819520"/>
+        <a:off x="237960" y="3380040"/>
+        <a:ext cx="5011200" cy="2819160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -953,9 +982,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>50760</xdr:colOff>
+      <xdr:colOff>50400</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -963,8 +992,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5413680" y="3171600"/>
-        <a:ext cx="4962240" cy="2791440"/>
+        <a:off x="5412600" y="3320640"/>
+        <a:ext cx="4959720" cy="2791080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -977,8 +1006,114 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -990,188 +1125,188 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="29.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="29.97"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="178.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <f aca="false">C2-B2</f>
         <v>25</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="5" t="n">
         <f aca="false">D2/B2</f>
         <v>2.5</v>
       </c>
-      <c r="F2" s="3" t="str">
+      <c r="F2" s="4" t="str">
         <f aca="false">IF(E2&gt;2.4,"Gyors","Lassú")</f>
         <v>Gyors</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="7" t="n">
         <f aca="false">SUM(D2:D6)</f>
         <v>195</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <f aca="false">C3-B3</f>
         <v>28</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="5" t="n">
         <f aca="false">D3/B3</f>
         <v>2.33333333333333</v>
       </c>
-      <c r="F3" s="3" t="str">
+      <c r="F3" s="4" t="str">
         <f aca="false">IF(E3&gt;2.4,"Gyors","Lassú")</f>
         <v>Lassú</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="6" t="n">
+      <c r="I3" s="7" t="n">
         <f aca="false">AVERAGE(D2:D6)</f>
         <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <f aca="false">C4-B4</f>
         <v>45</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="5" t="n">
         <f aca="false">D4/B4</f>
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="str">
+      <c r="F4" s="4" t="str">
         <f aca="false">IF(E4&gt;2.4,"Gyors","Lassú")</f>
         <v>Gyors</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="7" t="n">
+      <c r="I4" s="8" t="n">
         <f aca="false">MAX(E2:E6)</f>
         <v>3.25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
         <v>85</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <f aca="false">C5-B5</f>
         <v>65</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <f aca="false">D5/B5</f>
         <v>3.25</v>
       </c>
-      <c r="F5" s="3" t="str">
+      <c r="F5" s="4" t="str">
         <f aca="false">IF(E5&gt;2.4,"Gyors","Lassú")</f>
         <v>Gyors</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="8" t="n">
         <f aca="false">MIN(E2:E6)</f>
         <v>1.77777777777778</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <f aca="false">C6-B6</f>
         <v>32</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="5" t="n">
         <f aca="false">D6/B6</f>
         <v>1.77777777777778</v>
       </c>
-      <c r="F6" s="3" t="str">
+      <c r="F6" s="4" t="str">
         <f aca="false">IF(E6&gt;2.4,"Gyors","Lassú")</f>
         <v>Lassú</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="8" t="str">
+      <c r="I6" s="1" t="str">
         <f aca="false">INDEX($A$2:$A$6,MATCH(I4,$E$2:$E$6,0),1)</f>
         <v>Napraforgó</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="8" t="str">
+      <c r="I7" s="1" t="str">
         <f aca="false">INDEX($A$2:$A$6,MATCH(I5,$E$2:$E$6,0),1)</f>
         <v>Búza</v>
       </c>
@@ -1189,7 +1324,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1201,234 +1336,234 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <f aca="false">ROUND(E2*$B$18,0)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <f aca="false">F3-1</f>
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="9" t="n">
         <v>0.4</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <f aca="false">ROUND(E3*$B$18,0)</f>
         <v>12</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <f aca="false">F4-1</f>
         <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="9" t="n">
         <v>0.6</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <f aca="false">ROUND(E4*$B$18,0)</f>
         <v>18</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <f aca="false">F5-1</f>
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E5" s="9" t="n">
         <v>0.7</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <f aca="false">ROUND(E5*$B$18,0)</f>
         <v>21</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <f aca="false">F6-1</f>
         <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E6" s="9" t="n">
         <v>0.85</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <f aca="false">ROUND(E6*$B$18,0)</f>
         <v>26</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <f aca="false">B18</f>
         <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <f aca="false">SUM(B2:B15)</f>
         <v>30</v>
       </c>

</xml_diff>